<commit_message>
[doc] (journal travail) update journal de travil ops
</commit_message>
<xml_diff>
--- a/docs/Journal-de-Travail_Ops_BelkhiriaSofiene.xlsx
+++ b/docs/Journal-de-Travail_Ops_BelkhiriaSofiene.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\Install_in_NutShell\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1185B1F-19DF-4D92-ACB1-1D7D2BC2CA25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7054416F-AB1E-4B03-8B90-E0D8FAF78F91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>Remise de la partie dev du projet par le prof</t>
+  </si>
+  <si>
+    <t>Workflow push db</t>
   </si>
 </sst>
 </file>
@@ -1081,7 +1084,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>4.1666666666666664E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2012,7 +2015,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2065,7 +2068,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 0 heurs 25 minutes</v>
+        <v>0 jours 1 heurs 25 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2080,7 +2083,7 @@
       <c r="B4" s="5"/>
       <c r="C4" s="23">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
@@ -2088,7 +2091,7 @@
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2143,15 +2146,23 @@
       <c r="G7" s="15"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="str">
+      <c r="A8" s="8">
         <f>IF(ISBLANK(B8),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B8))</f>
-        <v/>
-      </c>
-      <c r="B8" s="47"/>
-      <c r="C8" s="48"/>
+        <v>51</v>
+      </c>
+      <c r="B8" s="47">
+        <v>45644</v>
+      </c>
+      <c r="C8" s="48">
+        <v>1</v>
+      </c>
       <c r="D8" s="49"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="37"/>
+      <c r="E8" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="37" t="s">
+        <v>30</v>
+      </c>
       <c r="G8" s="16"/>
       <c r="M8" t="s">
         <v>3</v>
@@ -8626,7 +8637,7 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
@@ -8638,7 +8649,7 @@
       </c>
       <c r="D5" s="34">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8747,7 +8758,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>1.7361111111111112E-2</v>
+        <v>5.9027777777777776E-2</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8984,6 +8995,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -8992,15 +9012,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9023,6 +9034,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9031,12 +9050,4 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[doc] (journal de travail ops) Update journal de travail
</commit_message>
<xml_diff>
--- a/docs/Journal-de-Travail_Ops_BelkhiriaSofiene.xlsx
+++ b/docs/Journal-de-Travail_Ops_BelkhiriaSofiene.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po66qga\Documents\GitHub\Install_in_NutShell\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7054416F-AB1E-4B03-8B90-E0D8FAF78F91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF1955A-EECD-4557-AB8A-7C48CB1825F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -134,6 +134,12 @@
   </si>
   <si>
     <t>Workflow push db</t>
+  </si>
+  <si>
+    <t>Ecriture de l'introduction + objectif de la doc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finalisation du workflow db push </t>
   </si>
 </sst>
 </file>
@@ -1084,13 +1090,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.1666666666666664E-2</c:v>
+                  <c:v>5.5555555555555552E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>6.25E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1.7361111111111112E-2</c:v>
@@ -2015,7 +2021,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2068,7 +2074,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 1 heurs 25 minutes</v>
+        <v>0 jours 3 heurs 15 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2083,15 +2089,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="23">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>85</v>
+        <v>195</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2175,15 +2181,25 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="str">
+      <c r="A9" s="17">
         <f>IF(ISBLANK(B9),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B9))</f>
-        <v/>
-      </c>
-      <c r="B9" s="51"/>
-      <c r="C9" s="52"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="37"/>
+        <v>51</v>
+      </c>
+      <c r="B9" s="51">
+        <v>45644</v>
+      </c>
+      <c r="C9" s="52">
+        <v>1</v>
+      </c>
+      <c r="D9" s="53">
+        <v>30</v>
+      </c>
+      <c r="E9" s="54" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="37" t="s">
+        <v>31</v>
+      </c>
       <c r="G9" s="18"/>
       <c r="M9" t="s">
         <v>4</v>
@@ -2196,15 +2212,23 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="str">
+      <c r="A10" s="8">
         <f>IF(ISBLANK(B10),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B10))</f>
-        <v/>
-      </c>
-      <c r="B10" s="47"/>
+        <v>51</v>
+      </c>
+      <c r="B10" s="47">
+        <v>45645</v>
+      </c>
       <c r="C10" s="48"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="37"/>
+      <c r="D10" s="49">
+        <v>20</v>
+      </c>
+      <c r="E10" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="37" t="s">
+        <v>32</v>
+      </c>
       <c r="G10" s="16"/>
       <c r="M10" t="s">
         <v>5</v>
@@ -8641,7 +8665,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C5" s="42" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8649,7 +8673,7 @@
       </c>
       <c r="D5" s="34">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>4.1666666666666664E-2</v>
+        <v>5.5555555555555552E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8673,11 +8697,11 @@
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C7" s="28" t="str">
         <f>'Journal de travail'!M11</f>
@@ -8685,7 +8709,7 @@
       </c>
       <c r="D7" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -8758,7 +8782,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>5.9027777777777776E-2</v>
+        <v>0.13541666666666666</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8995,15 +9019,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -9012,6 +9027,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9034,14 +9058,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9050,4 +9066,12 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>